<commit_message>
v02 - add tile bitmaps
</commit_message>
<xml_diff>
--- a/tiles.xlsx
+++ b/tiles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\MASTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F729626-4C8E-4DD0-B51B-67EEC5991A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FFA044-ABFD-4CA3-A5FA-55762021F875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="7275" windowWidth="24225" windowHeight="8310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="5595" windowWidth="24225" windowHeight="8310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
   <si>
     <t>TILE</t>
   </si>
@@ -111,12 +111,6 @@
     <t>000111000</t>
   </si>
   <si>
-    <t>Gras, Wald, Berg, BergSchnee</t>
-  </si>
-  <si>
-    <t>011000011</t>
-  </si>
-  <si>
     <t>111000000</t>
   </si>
   <si>
@@ -126,25 +120,25 @@
     <t>001001111</t>
   </si>
   <si>
-    <t>Gras, Wald</t>
-  </si>
-  <si>
-    <t>Wald, Gras, Kuh, Berg, Strand</t>
-  </si>
-  <si>
-    <t>Wasser, Gras, Strand, Wald</t>
-  </si>
-  <si>
-    <t>000011011</t>
-  </si>
-  <si>
     <t>Schnee</t>
   </si>
   <si>
     <t>Berg, Schnee, Schneemann</t>
   </si>
   <si>
-    <t>Gras, Wald, Berg, Schnee</t>
+    <t>Wald, Gras</t>
+  </si>
+  <si>
+    <t>Gras, Berg, Schnee</t>
+  </si>
+  <si>
+    <t>011000001</t>
+  </si>
+  <si>
+    <t>Wasser, Gras, Strand</t>
+  </si>
+  <si>
+    <t>000011001</t>
   </si>
 </sst>
 </file>
@@ -475,7 +469,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,28 +523,28 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -561,28 +555,28 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -593,28 +587,28 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -625,28 +619,28 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
       <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
         <v>36</v>
       </c>
-      <c r="G5" t="s">
-        <v>35</v>
-      </c>
       <c r="H5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
         <v>36</v>
       </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -721,28 +715,28 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="I8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -750,31 +744,31 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -785,25 +779,25 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>20</v>

</xml_diff>